<commit_message>
sat moved in plus refact
</commit_message>
<xml_diff>
--- a/it/Lang/lang.xlsx
+++ b/it/Lang/lang.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sandbox\it\lang\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Lab\sandbox\it\Lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7447835B-4B75-4437-BC14-AE2EDFEDB770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A71FFD-14C2-4120-8FE8-BFD45BC45D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lang" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,30 @@
     <sheet name="AI" sheetId="6" r:id="rId4"/>
     <sheet name="Text" sheetId="5" r:id="rId5"/>
     <sheet name="Popularity" sheetId="4" r:id="rId6"/>
+    <sheet name="Tiobe" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="96">
   <si>
     <t>Java</t>
   </si>
@@ -255,6 +267,69 @@
   </si>
   <si>
     <t>Not much</t>
+  </si>
+  <si>
+    <t>Nyelv</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Scientific</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Visual Basic</t>
+  </si>
+  <si>
+    <t>Delphi</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Fortran</t>
+  </si>
+  <si>
+    <t>Scratch</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Ada</t>
+  </si>
+  <si>
+    <t>MATLAB</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Perl</t>
+  </si>
+  <si>
+    <t>Cobol</t>
   </si>
 </sst>
 </file>
@@ -297,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +394,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -371,6 +452,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -655,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1268,4 +1356,294 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8C0B2A-330F-42A4-8484-2D96E88CF1DC}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="2.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6328125" style="2" customWidth="1"/>
+    <col min="3" max="6" width="8.7265625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="14">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="14">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="14">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="14">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="14">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="14">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="14">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="14">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="14">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="14">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="14">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C22" s="16">
+        <f>COUNTA(C2:C21)</f>
+        <v>7</v>
+      </c>
+      <c r="D22" s="16">
+        <f t="shared" ref="D22:F22" si="0">COUNTA(D2:D21)</f>
+        <v>7</v>
+      </c>
+      <c r="E22" s="16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>